<commit_message>
Added new Test classes
</commit_message>
<xml_diff>
--- a/src/main/java/com/projectname/qa/testdata/testdata.xlsx
+++ b/src/main/java/com/projectname/qa/testdata/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nigorabowles/eclipse-workspace/ProjectSkeleton/src/main/java/com/projectname/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFA1042-E8E1-9A49-91DB-2BBFE8038C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE01B66E-9A64-E84A-ADE0-4F45B23EE7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16840" activeTab="1" xr2:uid="{53EE145C-4D14-6B4A-996A-645144FC8C5D}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16840" xr2:uid="{53EE145C-4D14-6B4A-996A-645144FC8C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Email</t>
   </si>
@@ -73,13 +73,19 @@
   </si>
   <si>
     <t>Product Quality Concern - Order #</t>
+  </si>
+  <si>
+    <t>qa.test3@gmail.com</t>
+  </si>
+  <si>
+    <t>validPassword@456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,6 +131,20 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333399"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333399"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -166,6 +186,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E2433D-96C3-5740-A55C-65C5814BA9AD}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,6 +531,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -518,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005030D3-35DD-A845-828C-4F0C5F4616DC}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>